<commit_message>
Atualizado campo dos colaboradores
</commit_message>
<xml_diff>
--- a/1- Arquivos de entrada/Lista.xlsx
+++ b/1- Arquivos de entrada/Lista.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Almoxarifado\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desenv. Pessoal\1- Arquivos de entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D048723F-2443-492D-970A-98E2F1999C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C20B93C-92C0-4E28-830D-C5474FC34B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3C94BC27-CE5E-414A-A26A-BAB1BAD8CB68}"/>
   </bookViews>
@@ -27,32 +27,32 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>ADIVALDO NERO DE SOUZA</t>
-  </si>
-  <si>
-    <t>AGEU DE MATOS MIGUEL</t>
-  </si>
-  <si>
-    <t>ALAN JONATHAN PEREIRA</t>
-  </si>
-  <si>
-    <t>ADRIEL DA SILVA MONGE DE FREITAS</t>
-  </si>
-  <si>
-    <t>ADRIEL ANTONIO FAUSTINO QUEIROZ</t>
-  </si>
-  <si>
     <t>Matricula</t>
   </si>
   <si>
     <t>Nome</t>
+  </si>
+  <si>
+    <t>FUNCIONÁRIO 1</t>
+  </si>
+  <si>
+    <t>FUNCIONÁRIO 2</t>
+  </si>
+  <si>
+    <t>FUNCIONÁRIO 3</t>
+  </si>
+  <si>
+    <t>FUNCIONÁRIO 4</t>
+  </si>
+  <si>
+    <t>FUNCIONÁRIO 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +72,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -419,7 +425,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD106"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,10 +436,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -441,7 +447,7 @@
         <v>188</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,7 +455,7 @@
         <v>319</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -457,7 +463,7 @@
         <v>567</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -465,7 +471,7 @@
         <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -473,7 +479,7 @@
         <v>358</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -481,6 +487,7 @@
       <c r="B7" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>

</xml_diff>